<commit_message>
fix weekly get cast unsigned count
</commit_message>
<xml_diff>
--- a/public/Format_Timesheet.xlsx
+++ b/public/Format_Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59399471-A498-483D-B9F9-7EBB047DCC52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456AC27C-1013-480C-90F6-94AD2D4656F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,10 +75,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="165" formatCode="d&quot;日&quot;"/>
-    <numFmt numFmtId="166" formatCode="yyyy&quot;年&quot;m&quot;月&quot;dd&quot;日&quot;"/>
-    <numFmt numFmtId="167" formatCode="[Red][=1]aaa;[Blue][=7]aaa;aaa"/>
-    <numFmt numFmtId="168" formatCode="[h]:mm"/>
+    <numFmt numFmtId="164" formatCode="d&quot;日&quot;"/>
+    <numFmt numFmtId="165" formatCode="yyyy&quot;年&quot;m&quot;月&quot;dd&quot;日&quot;"/>
+    <numFmt numFmtId="166" formatCode="[Red][=1]aaa;[Blue][=7]aaa;aaa"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -344,7 +344,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -382,13 +382,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -409,10 +409,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -424,7 +424,13 @@
     <xf numFmtId="20" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -958,7 +964,7 @@
   <dimension ref="B1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -984,6 +990,7 @@
       <c r="B2" s="14">
         <v>43831</v>
       </c>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:10" ht="19.2" customHeight="1">
       <c r="B3" s="5" t="s">
@@ -1500,9 +1507,7 @@
     <row r="34" spans="2:10" ht="21.6" customHeight="1" thickTop="1">
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
-      <c r="D34" s="19">
-        <v>22</v>
-      </c>
+      <c r="D34" s="19"/>
       <c r="E34" s="20" t="s">
         <v>11</v>
       </c>
@@ -1530,21 +1535,15 @@
         <v>12</v>
       </c>
       <c r="C38" s="11"/>
-      <c r="D38" s="11">
-        <v>165</v>
-      </c>
+      <c r="D38" s="28"/>
       <c r="E38" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="11">
-        <v>176</v>
-      </c>
+      <c r="F38" s="28"/>
       <c r="G38" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H38" s="11">
-        <v>11</v>
-      </c>
+      <c r="H38" s="29"/>
       <c r="I38" s="12"/>
       <c r="J38" s="9"/>
     </row>

</xml_diff>